<commit_message>
Caricata prima versione senza classi e senza lettura file pdf
</commit_message>
<xml_diff>
--- a/test/test_due/Cartella.xlsx
+++ b/test/test_due/Cartella.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescaronci/Desktop/Programmazione/ESERCIZIO_FILESYSTEM/test/test_due/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A9846-5308-6144-A014-3B98F5561C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ED2D7E-4430-C848-9324-DE000980C976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="28040" windowHeight="16580" xr2:uid="{4A61DE26-DB17-B342-8072-5CBD045A4D6F}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{4A61DE26-DB17-B342-8072-5CBD045A4D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Gaia, Francesca</t>
   </si>
@@ -45,10 +45,13 @@
     <t>Gruppo due</t>
   </si>
   <si>
-    <t>Progetto uno</t>
-  </si>
-  <si>
-    <t>Progetto due</t>
+    <t>docente</t>
+  </si>
+  <si>
+    <t>progetto uno</t>
+  </si>
+  <si>
+    <t>progetto due</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1DD499-9407-1441-89B7-137ABFED87CF}">
-  <dimension ref="B1:D3"/>
+  <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -418,10 +421,10 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -433,6 +436,11 @@
       </c>
       <c r="D3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>